<commit_message>
States not defined in publication → ?
</commit_message>
<xml_diff>
--- a/Project4790_C. E. Mitchell(2013).xlsx
+++ b/Project4790_C. E. Mitchell(2013).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remi/Desktop/Finished &amp; Uploaded copy 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjg18\GitHub\neotrans\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8BE279-29C9-B742-A74F-F75850CDFE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DC8E2C-C7AA-4571-8758-D108DD7FCF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{82CB97C3-56FC-3A46-9CD0-A600CD051AFF}"/>
+    <workbookView xWindow="-15" yWindow="7080" windowWidth="15870" windowHeight="18585" xr2:uid="{82CB97C3-56FC-3A46-9CD0-A600CD051AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Project4790" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Charlabels</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>NT?;0=0-;1=11;2=12;3=13</t>
+  </si>
+  <si>
+    <t>N;0=0;1=1;2=?</t>
+  </si>
+  <si>
+    <t>T;0=0;1=1;2=?</t>
   </si>
 </sst>
 </file>
@@ -607,16 +613,16 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.33203125" customWidth="1"/>
-    <col min="2" max="3" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="83.375" customWidth="1"/>
+    <col min="2" max="3" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,18 +633,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -646,7 +652,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -654,18 +660,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>35</v>
+      <c r="B5" t="s">
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -676,7 +682,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -687,7 +693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -698,7 +704,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -709,18 +715,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
+      <c r="B10" t="s">
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -731,18 +737,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
+      <c r="B12" t="s">
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -753,18 +759,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>35</v>
+      <c r="B14" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -775,7 +781,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -786,7 +792,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -797,7 +803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -805,18 +811,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
+      <c r="B19" t="s">
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -827,18 +833,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>35</v>
+      <c r="B21" t="s">
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -849,7 +855,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -860,18 +866,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>38</v>
+      <c r="B24" t="s">
+        <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -882,7 +888,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -890,18 +896,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>35</v>
+      <c r="B27" t="s">
+        <v>42</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -912,7 +918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -923,7 +929,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -934,7 +940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -942,18 +948,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
+      <c r="B32" t="s">
+        <v>42</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>

</xml_diff>